<commit_message>
Queue page and statistics page
</commit_message>
<xml_diff>
--- a/dataHistory.xlsx
+++ b/dataHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan_markvart\Documents\Python\Projects\InteractiveDashBoadr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D4E400-131F-47C0-B1BF-F70D07F5B2E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3784C506-E292-464D-86A1-6D58B6A1DA2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$C$999</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$C$1001</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2997" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3028" uniqueCount="42">
   <si>
     <t>21</t>
   </si>
@@ -140,6 +140,15 @@
   </si>
   <si>
     <t>VIS3xx</t>
+  </si>
+  <si>
+    <t>VIS340</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CM220 </t>
+  </si>
+  <si>
+    <t>VIS220</t>
   </si>
 </sst>
 </file>
@@ -542,10 +551,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C999"/>
+  <dimension ref="A1:C1030"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F225" sqref="F225"/>
+    <sheetView tabSelected="1" topLeftCell="A908" workbookViewId="0">
+      <selection activeCell="B1002" sqref="B1002:B1030"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -649,7 +658,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1232,7 +1241,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>2</v>
       </c>
@@ -1243,7 +1252,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>2</v>
       </c>
@@ -1254,7 +1263,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>2</v>
       </c>
@@ -1265,7 +1274,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>2</v>
       </c>
@@ -1276,7 +1285,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>2</v>
       </c>
@@ -1287,7 +1296,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>2</v>
       </c>
@@ -1298,7 +1307,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>2</v>
       </c>
@@ -1309,7 +1318,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>2</v>
       </c>
@@ -1320,7 +1329,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>2</v>
       </c>
@@ -1331,7 +1340,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>2</v>
       </c>
@@ -1342,7 +1351,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>2</v>
       </c>
@@ -1353,7 +1362,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>2</v>
       </c>
@@ -1364,7 +1373,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>2</v>
       </c>
@@ -1375,7 +1384,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>2</v>
       </c>
@@ -1386,7 +1395,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>2</v>
       </c>
@@ -1397,7 +1406,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>2</v>
       </c>
@@ -1408,7 +1417,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>2</v>
       </c>
@@ -1419,7 +1428,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>2</v>
       </c>
@@ -1430,7 +1439,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>2</v>
       </c>
@@ -1441,7 +1450,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>2</v>
       </c>
@@ -1452,7 +1461,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>2</v>
       </c>
@@ -1463,7 +1472,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>2</v>
       </c>
@@ -1474,7 +1483,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>2</v>
       </c>
@@ -1485,7 +1494,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>2</v>
       </c>
@@ -1496,7 +1505,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="87" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>2</v>
       </c>
@@ -1507,18 +1516,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B88" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C88" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="89" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>2</v>
       </c>
@@ -1529,7 +1538,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="90" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>2</v>
       </c>
@@ -1540,7 +1549,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="91" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>2</v>
       </c>
@@ -1551,7 +1560,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>2</v>
       </c>
@@ -1562,7 +1571,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="93" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>2</v>
       </c>
@@ -1573,7 +1582,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="94" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>2</v>
       </c>
@@ -1584,7 +1593,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="95" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>2</v>
       </c>
@@ -1595,7 +1604,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="96" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>2</v>
       </c>
@@ -1606,7 +1615,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>2</v>
       </c>
@@ -1617,7 +1626,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>2</v>
       </c>
@@ -1628,7 +1637,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="99" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>2</v>
       </c>
@@ -2024,12 +2033,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>1</v>
       </c>
       <c r="B135" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C135" t="s">
         <v>38</v>
@@ -2508,7 +2517,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="179" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>2</v>
       </c>
@@ -2519,7 +2528,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="180" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>2</v>
       </c>
@@ -2530,7 +2539,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="181" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>2</v>
       </c>
@@ -2541,7 +2550,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="182" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>2</v>
       </c>
@@ -2552,7 +2561,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="183" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>2</v>
       </c>
@@ -2563,7 +2572,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="184" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>2</v>
       </c>
@@ -2574,7 +2583,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="185" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>2</v>
       </c>
@@ -2585,7 +2594,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="186" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>2</v>
       </c>
@@ -2596,7 +2605,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="187" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>2</v>
       </c>
@@ -2607,7 +2616,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="188" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>2</v>
       </c>
@@ -2618,7 +2627,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="189" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>2</v>
       </c>
@@ -2629,7 +2638,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="190" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>2</v>
       </c>
@@ -2640,7 +2649,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="191" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>2</v>
       </c>
@@ -2651,7 +2660,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="192" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>2</v>
       </c>
@@ -2662,7 +2671,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="193" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>2</v>
       </c>
@@ -2673,7 +2682,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="194" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>2</v>
       </c>
@@ -2684,7 +2693,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="195" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>2</v>
       </c>
@@ -2695,7 +2704,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="196" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>2</v>
       </c>
@@ -2706,7 +2715,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="197" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>2</v>
       </c>
@@ -2717,7 +2726,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="198" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>2</v>
       </c>
@@ -2728,7 +2737,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="199" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>2</v>
       </c>
@@ -2739,7 +2748,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="200" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>2</v>
       </c>
@@ -2750,7 +2759,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="201" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>2</v>
       </c>
@@ -2761,7 +2770,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="202" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>2</v>
       </c>
@@ -2772,7 +2781,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="203" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>2</v>
       </c>
@@ -2783,7 +2792,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="204" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>2</v>
       </c>
@@ -2794,7 +2803,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="205" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>2</v>
       </c>
@@ -2805,7 +2814,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="206" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>2</v>
       </c>
@@ -2816,7 +2825,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="207" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>2</v>
       </c>
@@ -3014,12 +3023,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>1</v>
       </c>
       <c r="B225" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C225" t="s">
         <v>38</v>
@@ -3113,12 +3122,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B234" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C234" t="s">
         <v>38</v>
@@ -3366,7 +3375,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="257" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>2</v>
       </c>
@@ -3377,7 +3386,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="258" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>2</v>
       </c>
@@ -3388,7 +3397,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="259" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>2</v>
       </c>
@@ -3399,7 +3408,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="260" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>2</v>
       </c>
@@ -3410,7 +3419,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="261" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>2</v>
       </c>
@@ -3421,7 +3430,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="262" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>2</v>
       </c>
@@ -3432,7 +3441,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="263" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>2</v>
       </c>
@@ -3443,7 +3452,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="264" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>2</v>
       </c>
@@ -3454,7 +3463,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="265" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>2</v>
       </c>
@@ -3465,7 +3474,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="266" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>2</v>
       </c>
@@ -3476,7 +3485,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="267" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>2</v>
       </c>
@@ -3487,7 +3496,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="268" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>2</v>
       </c>
@@ -3498,29 +3507,29 @@
         <v>20</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B269" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C269" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B270" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C270" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="271" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>2</v>
       </c>
@@ -3531,7 +3540,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="272" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>2</v>
       </c>
@@ -3542,7 +3551,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="273" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>2</v>
       </c>
@@ -3553,7 +3562,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="274" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>2</v>
       </c>
@@ -3564,7 +3573,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="275" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>2</v>
       </c>
@@ -3575,7 +3584,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="276" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>2</v>
       </c>
@@ -3586,7 +3595,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="277" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>2</v>
       </c>
@@ -3597,7 +3606,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="278" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>2</v>
       </c>
@@ -3608,7 +3617,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="279" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>2</v>
       </c>
@@ -3619,7 +3628,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="280" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>2</v>
       </c>
@@ -3630,7 +3639,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="281" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>2</v>
       </c>
@@ -3641,7 +3650,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="282" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>2</v>
       </c>
@@ -3652,7 +3661,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="283" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>2</v>
       </c>
@@ -3663,7 +3672,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="284" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>2</v>
       </c>
@@ -3861,12 +3870,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>1</v>
       </c>
       <c r="B302" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C302" t="s">
         <v>38</v>
@@ -3960,12 +3969,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B311" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C311" t="s">
         <v>38</v>
@@ -4081,12 +4090,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B322" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C322" t="s">
         <v>38</v>
@@ -4103,7 +4112,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="324" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>2</v>
       </c>
@@ -4114,7 +4123,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="325" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>2</v>
       </c>
@@ -4125,7 +4134,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="326" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>2</v>
       </c>
@@ -4136,18 +4145,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B327" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C327" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="328" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>2</v>
       </c>
@@ -4158,7 +4167,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="329" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>2</v>
       </c>
@@ -4169,7 +4178,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="330" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>2</v>
       </c>
@@ -4180,7 +4189,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="331" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>2</v>
       </c>
@@ -4191,7 +4200,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="332" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>2</v>
       </c>
@@ -4202,7 +4211,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="333" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>2</v>
       </c>
@@ -4213,7 +4222,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="334" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>2</v>
       </c>
@@ -4224,7 +4233,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="335" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>2</v>
       </c>
@@ -4235,7 +4244,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="336" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>2</v>
       </c>
@@ -4246,7 +4255,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="337" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>2</v>
       </c>
@@ -4257,7 +4266,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="338" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>2</v>
       </c>
@@ -4268,7 +4277,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="339" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>2</v>
       </c>
@@ -4279,7 +4288,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="340" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>2</v>
       </c>
@@ -4356,12 +4365,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>1</v>
       </c>
       <c r="B347" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C347" t="s">
         <v>38</v>
@@ -4642,12 +4651,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B373" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C373" t="s">
         <v>38</v>
@@ -4840,12 +4849,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="391" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B391" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C391" t="s">
         <v>38</v>
@@ -4862,7 +4871,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="393" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
         <v>2</v>
       </c>
@@ -4873,7 +4882,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="394" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
         <v>2</v>
       </c>
@@ -4884,7 +4893,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="395" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
         <v>2</v>
       </c>
@@ -4895,7 +4904,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="396" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
         <v>2</v>
       </c>
@@ -4906,7 +4915,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="397" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
         <v>2</v>
       </c>
@@ -4917,7 +4926,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="398" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
         <v>2</v>
       </c>
@@ -4928,7 +4937,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="399" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
         <v>2</v>
       </c>
@@ -4939,7 +4948,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="400" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
         <v>2</v>
       </c>
@@ -4950,7 +4959,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="401" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>2</v>
       </c>
@@ -4961,7 +4970,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="402" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
         <v>2</v>
       </c>
@@ -4972,7 +4981,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="403" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>2</v>
       </c>
@@ -4983,7 +4992,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="404" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
         <v>2</v>
       </c>
@@ -4994,7 +5003,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="405" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>2</v>
       </c>
@@ -5005,7 +5014,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="406" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
         <v>2</v>
       </c>
@@ -5016,7 +5025,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="407" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
         <v>2</v>
       </c>
@@ -5027,7 +5036,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="408" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
         <v>2</v>
       </c>
@@ -5038,7 +5047,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="409" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
         <v>2</v>
       </c>
@@ -5049,7 +5058,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="410" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
         <v>2</v>
       </c>
@@ -5060,7 +5069,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="411" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
         <v>2</v>
       </c>
@@ -5071,7 +5080,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="412" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
         <v>2</v>
       </c>
@@ -5082,7 +5091,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="413" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
         <v>2</v>
       </c>
@@ -5093,7 +5102,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="414" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
         <v>2</v>
       </c>
@@ -5104,7 +5113,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="415" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
         <v>2</v>
       </c>
@@ -5115,7 +5124,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="416" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
         <v>2</v>
       </c>
@@ -5126,7 +5135,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="417" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
         <v>2</v>
       </c>
@@ -5137,7 +5146,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="418" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
         <v>2</v>
       </c>
@@ -5148,7 +5157,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="419" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
         <v>2</v>
       </c>
@@ -5159,7 +5168,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="420" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A420" t="s">
         <v>2</v>
       </c>
@@ -5170,7 +5179,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="421" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A421" t="s">
         <v>2</v>
       </c>
@@ -5588,12 +5597,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="459" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A459" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B459" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C459" t="s">
         <v>38</v>
@@ -5797,7 +5806,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="478" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A478" t="s">
         <v>2</v>
       </c>
@@ -5808,7 +5817,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="479" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A479" t="s">
         <v>2</v>
       </c>
@@ -5819,7 +5828,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="480" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A480" t="s">
         <v>2</v>
       </c>
@@ -5830,7 +5839,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="481" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A481" t="s">
         <v>2</v>
       </c>
@@ -5841,7 +5850,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="482" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A482" t="s">
         <v>2</v>
       </c>
@@ -5852,18 +5861,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="483" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A483" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B483" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C483" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="484" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A484" t="s">
         <v>2</v>
       </c>
@@ -5874,7 +5883,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="485" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A485" t="s">
         <v>2</v>
       </c>
@@ -5885,7 +5894,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="486" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A486" t="s">
         <v>2</v>
       </c>
@@ -5896,7 +5905,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="487" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A487" t="s">
         <v>2</v>
       </c>
@@ -5907,7 +5916,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="488" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A488" t="s">
         <v>2</v>
       </c>
@@ -5918,29 +5927,29 @@
         <v>20</v>
       </c>
     </row>
-    <row r="489" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A489" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B489" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C489" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="490" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A490" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B490" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C490" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="491" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A491" t="s">
         <v>2</v>
       </c>
@@ -5951,7 +5960,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="492" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A492" t="s">
         <v>2</v>
       </c>
@@ -5962,7 +5971,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="493" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A493" t="s">
         <v>2</v>
       </c>
@@ -5973,7 +5982,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="494" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A494" t="s">
         <v>2</v>
       </c>
@@ -5984,7 +5993,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="495" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A495" t="s">
         <v>2</v>
       </c>
@@ -5995,7 +6004,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="496" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A496" t="s">
         <v>2</v>
       </c>
@@ -6006,7 +6015,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="497" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
         <v>2</v>
       </c>
@@ -6017,7 +6026,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="498" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A498" t="s">
         <v>2</v>
       </c>
@@ -6028,7 +6037,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="499" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A499" t="s">
         <v>2</v>
       </c>
@@ -6039,7 +6048,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="500" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A500" t="s">
         <v>2</v>
       </c>
@@ -6050,7 +6059,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="501" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A501" t="s">
         <v>2</v>
       </c>
@@ -6061,7 +6070,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="502" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="502" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A502" t="s">
         <v>2</v>
       </c>
@@ -6072,7 +6081,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="503" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A503" t="s">
         <v>2</v>
       </c>
@@ -6083,7 +6092,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="504" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="504" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A504" t="s">
         <v>2</v>
       </c>
@@ -6094,7 +6103,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="505" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A505" t="s">
         <v>2</v>
       </c>
@@ -6105,7 +6114,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="506" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="506" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A506" t="s">
         <v>2</v>
       </c>
@@ -6116,7 +6125,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="507" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="507" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A507" t="s">
         <v>2</v>
       </c>
@@ -6127,7 +6136,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="508" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="508" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A508" t="s">
         <v>2</v>
       </c>
@@ -6138,7 +6147,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="509" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="509" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A509" t="s">
         <v>2</v>
       </c>
@@ -6149,7 +6158,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="510" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="510" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A510" t="s">
         <v>2</v>
       </c>
@@ -6160,7 +6169,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="511" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A511" t="s">
         <v>2</v>
       </c>
@@ -6171,7 +6180,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="512" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="512" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A512" t="s">
         <v>2</v>
       </c>
@@ -6182,7 +6191,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="513" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="513" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A513" t="s">
         <v>2</v>
       </c>
@@ -6193,7 +6202,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="514" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="514" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A514" t="s">
         <v>2</v>
       </c>
@@ -6204,7 +6213,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="515" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="515" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A515" t="s">
         <v>2</v>
       </c>
@@ -6413,12 +6422,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="534" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="534" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A534" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B534" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C534" t="s">
         <v>38</v>
@@ -6677,12 +6686,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="558" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="558" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A558" t="s">
         <v>0</v>
       </c>
       <c r="B558" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C558" t="s">
         <v>38</v>
@@ -6710,12 +6719,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="561" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="561" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A561" t="s">
         <v>0</v>
       </c>
       <c r="B561" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C561" t="s">
         <v>38</v>
@@ -6875,7 +6884,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="576" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="576" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A576" t="s">
         <v>2</v>
       </c>
@@ -6886,18 +6895,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="577" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="577" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A577" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B577" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C577" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="578" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="578" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A578" t="s">
         <v>2</v>
       </c>
@@ -6908,7 +6917,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="579" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="579" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A579" t="s">
         <v>2</v>
       </c>
@@ -6919,7 +6928,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="580" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="580" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A580" t="s">
         <v>2</v>
       </c>
@@ -6930,7 +6939,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="581" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="581" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A581" t="s">
         <v>2</v>
       </c>
@@ -6941,7 +6950,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="582" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="582" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A582" t="s">
         <v>2</v>
       </c>
@@ -6952,7 +6961,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="583" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="583" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A583" t="s">
         <v>2</v>
       </c>
@@ -6963,7 +6972,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="584" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="584" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A584" t="s">
         <v>2</v>
       </c>
@@ -6974,7 +6983,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="585" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="585" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A585" t="s">
         <v>2</v>
       </c>
@@ -6985,7 +6994,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="586" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="586" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A586" t="s">
         <v>2</v>
       </c>
@@ -6996,7 +7005,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="587" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="587" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A587" t="s">
         <v>2</v>
       </c>
@@ -7007,7 +7016,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="588" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="588" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A588" t="s">
         <v>2</v>
       </c>
@@ -7018,7 +7027,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="589" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="589" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A589" t="s">
         <v>2</v>
       </c>
@@ -7029,7 +7038,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="590" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="590" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A590" t="s">
         <v>2</v>
       </c>
@@ -7040,7 +7049,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="591" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="591" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A591" t="s">
         <v>2</v>
       </c>
@@ -7051,7 +7060,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="592" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="592" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A592" t="s">
         <v>2</v>
       </c>
@@ -7062,7 +7071,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="593" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="593" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A593" t="s">
         <v>2</v>
       </c>
@@ -7073,7 +7082,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="594" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="594" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A594" t="s">
         <v>2</v>
       </c>
@@ -7084,7 +7093,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="595" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="595" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A595" t="s">
         <v>2</v>
       </c>
@@ -7095,7 +7104,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="596" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="596" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A596" t="s">
         <v>2</v>
       </c>
@@ -7106,7 +7115,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="597" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="597" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A597" t="s">
         <v>2</v>
       </c>
@@ -7117,7 +7126,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="598" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="598" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A598" t="s">
         <v>2</v>
       </c>
@@ -7128,7 +7137,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="599" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="599" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A599" t="s">
         <v>2</v>
       </c>
@@ -7139,7 +7148,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="600" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="600" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A600" t="s">
         <v>2</v>
       </c>
@@ -7194,12 +7203,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="605" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="605" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A605" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B605" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C605" t="s">
         <v>38</v>
@@ -7370,12 +7379,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="621" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="621" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A621" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B621" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C621" t="s">
         <v>38</v>
@@ -7678,18 +7687,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="649" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="649" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A649" t="s">
         <v>0</v>
       </c>
       <c r="B649" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C649" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="650" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="650" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A650" t="s">
         <v>0</v>
       </c>
@@ -7755,7 +7764,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="656" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="656" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A656" t="s">
         <v>0</v>
       </c>
@@ -7766,7 +7775,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="657" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="657" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A657" t="s">
         <v>0</v>
       </c>
@@ -7865,7 +7874,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="666" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="666" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A666" t="s">
         <v>0</v>
       </c>
@@ -7898,7 +7907,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="669" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="669" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A669" t="s">
         <v>0</v>
       </c>
@@ -8140,7 +8149,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="691" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="691" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A691" t="s">
         <v>2</v>
       </c>
@@ -8151,7 +8160,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="692" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="692" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A692" t="s">
         <v>2</v>
       </c>
@@ -8162,7 +8171,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="693" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="693" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A693" t="s">
         <v>2</v>
       </c>
@@ -8173,7 +8182,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="694" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="694" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A694" t="s">
         <v>2</v>
       </c>
@@ -8184,7 +8193,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="695" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="695" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A695" t="s">
         <v>2</v>
       </c>
@@ -8195,7 +8204,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="696" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="696" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A696" t="s">
         <v>2</v>
       </c>
@@ -8206,7 +8215,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="697" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="697" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A697" t="s">
         <v>2</v>
       </c>
@@ -8217,7 +8226,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="698" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="698" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A698" t="s">
         <v>2</v>
       </c>
@@ -8228,7 +8237,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="699" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="699" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A699" t="s">
         <v>2</v>
       </c>
@@ -8239,7 +8248,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="700" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="700" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A700" t="s">
         <v>2</v>
       </c>
@@ -8250,7 +8259,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="701" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="701" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A701" t="s">
         <v>2</v>
       </c>
@@ -8261,7 +8270,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="702" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="702" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A702" t="s">
         <v>2</v>
       </c>
@@ -8272,7 +8281,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="703" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="703" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A703" t="s">
         <v>2</v>
       </c>
@@ -8283,7 +8292,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="704" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="704" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A704" t="s">
         <v>2</v>
       </c>
@@ -8294,7 +8303,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="705" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="705" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A705" t="s">
         <v>2</v>
       </c>
@@ -8305,7 +8314,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="706" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="706" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A706" t="s">
         <v>2</v>
       </c>
@@ -8316,7 +8325,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="707" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="707" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A707" t="s">
         <v>2</v>
       </c>
@@ -8327,7 +8336,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="708" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="708" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A708" t="s">
         <v>2</v>
       </c>
@@ -8338,7 +8347,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="709" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="709" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A709" t="s">
         <v>2</v>
       </c>
@@ -8349,7 +8358,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="710" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="710" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A710" t="s">
         <v>2</v>
       </c>
@@ -8360,7 +8369,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="711" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="711" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A711" t="s">
         <v>2</v>
       </c>
@@ -8371,7 +8380,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="712" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="712" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A712" t="s">
         <v>2</v>
       </c>
@@ -8382,7 +8391,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="713" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="713" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A713" t="s">
         <v>2</v>
       </c>
@@ -8393,7 +8402,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="714" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="714" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A714" t="s">
         <v>2</v>
       </c>
@@ -8404,7 +8413,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="715" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="715" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A715" t="s">
         <v>2</v>
       </c>
@@ -8415,7 +8424,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="716" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="716" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A716" t="s">
         <v>2</v>
       </c>
@@ -8426,9 +8435,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="717" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="717" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A717" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B717" t="s">
         <v>12</v>
@@ -8437,7 +8446,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="718" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="718" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A718" t="s">
         <v>2</v>
       </c>
@@ -8448,7 +8457,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="719" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="719" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A719" t="s">
         <v>2</v>
       </c>
@@ -8459,18 +8468,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="720" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="720" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A720" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B720" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C720" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="721" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="721" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A721" t="s">
         <v>2</v>
       </c>
@@ -8481,7 +8490,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="722" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="722" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A722" t="s">
         <v>2</v>
       </c>
@@ -8492,7 +8501,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="723" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="723" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A723" t="s">
         <v>2</v>
       </c>
@@ -8503,7 +8512,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="724" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="724" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A724" t="s">
         <v>2</v>
       </c>
@@ -8514,7 +8523,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="725" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="725" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A725" t="s">
         <v>2</v>
       </c>
@@ -8525,7 +8534,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="726" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="726" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A726" t="s">
         <v>2</v>
       </c>
@@ -8536,7 +8545,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="727" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="727" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A727" t="s">
         <v>2</v>
       </c>
@@ -8547,7 +8556,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="728" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="728" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A728" t="s">
         <v>2</v>
       </c>
@@ -8558,7 +8567,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="729" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="729" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A729" t="s">
         <v>2</v>
       </c>
@@ -8569,7 +8578,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="730" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="730" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A730" t="s">
         <v>2</v>
       </c>
@@ -8580,7 +8589,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="731" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="731" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A731" t="s">
         <v>2</v>
       </c>
@@ -8591,7 +8600,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="732" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="732" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A732" t="s">
         <v>2</v>
       </c>
@@ -8602,7 +8611,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="733" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="733" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A733" t="s">
         <v>2</v>
       </c>
@@ -8613,7 +8622,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="734" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="734" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A734" t="s">
         <v>2</v>
       </c>
@@ -8624,7 +8633,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="735" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="735" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A735" t="s">
         <v>2</v>
       </c>
@@ -8635,7 +8644,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="736" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="736" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A736" t="s">
         <v>2</v>
       </c>
@@ -8646,7 +8655,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="737" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="737" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A737" t="s">
         <v>2</v>
       </c>
@@ -8657,7 +8666,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="738" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="738" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A738" t="s">
         <v>2</v>
       </c>
@@ -8668,7 +8677,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="739" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="739" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A739" t="s">
         <v>2</v>
       </c>
@@ -8679,7 +8688,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="740" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="740" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A740" t="s">
         <v>2</v>
       </c>
@@ -8690,7 +8699,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="741" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="741" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A741" t="s">
         <v>2</v>
       </c>
@@ -8701,7 +8710,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="742" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="742" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A742" t="s">
         <v>2</v>
       </c>
@@ -8712,7 +8721,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="743" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="743" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A743" t="s">
         <v>2</v>
       </c>
@@ -8723,7 +8732,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="744" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="744" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A744" t="s">
         <v>2</v>
       </c>
@@ -8734,7 +8743,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="745" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="745" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A745" t="s">
         <v>2</v>
       </c>
@@ -8745,7 +8754,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="746" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="746" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A746" t="s">
         <v>2</v>
       </c>
@@ -8789,12 +8798,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="750" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="750" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A750" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B750" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C750" t="s">
         <v>38</v>
@@ -8888,23 +8897,23 @@
         <v>15</v>
       </c>
     </row>
-    <row r="759" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="759" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A759" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B759" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C759" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="760" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="760" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A760" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B760" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C760" t="s">
         <v>38</v>
@@ -9504,7 +9513,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="815" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="815" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A815" t="s">
         <v>2</v>
       </c>
@@ -9515,12 +9524,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="816" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="816" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A816" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B816" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C816" t="s">
         <v>38</v>
@@ -9531,13 +9540,13 @@
         <v>2</v>
       </c>
       <c r="B817" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C817" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="818" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="818" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A818" t="s">
         <v>2</v>
       </c>
@@ -9548,7 +9557,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="819" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="819" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A819" t="s">
         <v>2</v>
       </c>
@@ -9559,7 +9568,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="820" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="820" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A820" t="s">
         <v>2</v>
       </c>
@@ -9570,7 +9579,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="821" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="821" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A821" t="s">
         <v>2</v>
       </c>
@@ -9581,7 +9590,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="822" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="822" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A822" t="s">
         <v>2</v>
       </c>
@@ -9592,7 +9601,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="823" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="823" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A823" t="s">
         <v>2</v>
       </c>
@@ -9608,7 +9617,7 @@
         <v>2</v>
       </c>
       <c r="B824" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C824" t="s">
         <v>38</v>
@@ -9693,10 +9702,10 @@
     </row>
     <row r="832" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A832" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B832" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C832" t="s">
         <v>38</v>
@@ -9726,10 +9735,10 @@
     </row>
     <row r="835" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A835" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B835" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C835" t="s">
         <v>38</v>
@@ -10243,10 +10252,10 @@
     </row>
     <row r="882" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A882" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B882" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C882" t="s">
         <v>38</v>
@@ -10265,10 +10274,10 @@
     </row>
     <row r="884" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A884" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B884" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C884" t="s">
         <v>38</v>
@@ -10340,7 +10349,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="891" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="891" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A891" t="s">
         <v>2</v>
       </c>
@@ -10356,13 +10365,13 @@
         <v>2</v>
       </c>
       <c r="B892" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C892" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="893" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="893" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A893" t="s">
         <v>2</v>
       </c>
@@ -10373,7 +10382,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="894" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="894" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A894" t="s">
         <v>2</v>
       </c>
@@ -10384,7 +10393,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="895" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="895" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A895" t="s">
         <v>2</v>
       </c>
@@ -10395,7 +10404,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="896" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="896" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A896" t="s">
         <v>2</v>
       </c>
@@ -10411,7 +10420,7 @@
         <v>2</v>
       </c>
       <c r="B897" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C897" t="s">
         <v>38</v>
@@ -10422,13 +10431,13 @@
         <v>2</v>
       </c>
       <c r="B898" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C898" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="899" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="899" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A899" t="s">
         <v>2</v>
       </c>
@@ -10439,7 +10448,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="900" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="900" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A900" t="s">
         <v>2</v>
       </c>
@@ -10450,7 +10459,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="901" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="901" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A901" t="s">
         <v>2</v>
       </c>
@@ -10461,7 +10470,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="902" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="902" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A902" t="s">
         <v>2</v>
       </c>
@@ -10472,7 +10481,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="903" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="903" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A903" t="s">
         <v>2</v>
       </c>
@@ -10483,7 +10492,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="904" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="904" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A904" t="s">
         <v>2</v>
       </c>
@@ -10494,7 +10503,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="905" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="905" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A905" t="s">
         <v>2</v>
       </c>
@@ -10505,7 +10514,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="906" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="906" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A906" t="s">
         <v>2</v>
       </c>
@@ -10521,13 +10530,13 @@
         <v>2</v>
       </c>
       <c r="B907" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C907" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="908" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="908" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A908" t="s">
         <v>2</v>
       </c>
@@ -10538,7 +10547,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="909" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="909" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A909" t="s">
         <v>2</v>
       </c>
@@ -10554,13 +10563,13 @@
         <v>2</v>
       </c>
       <c r="B910" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C910" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="911" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="911" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A911" t="s">
         <v>2</v>
       </c>
@@ -10716,10 +10725,10 @@
     </row>
     <row r="925" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A925" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B925" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C925" t="s">
         <v>38</v>
@@ -10826,10 +10835,10 @@
     </row>
     <row r="935" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A935" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B935" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C935" t="s">
         <v>38</v>
@@ -10903,10 +10912,10 @@
     </row>
     <row r="942" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A942" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B942" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C942" t="s">
         <v>38</v>
@@ -10925,10 +10934,10 @@
     </row>
     <row r="944" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A944" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B944" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C944" t="s">
         <v>38</v>
@@ -11189,10 +11198,10 @@
     </row>
     <row r="968" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A968" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B968" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C968" t="s">
         <v>38</v>
@@ -11365,10 +11374,10 @@
     </row>
     <row r="984" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A984" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B984" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C984" t="s">
         <v>38</v>
@@ -11409,10 +11418,10 @@
     </row>
     <row r="988" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A988" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B988" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C988" t="s">
         <v>38</v>
@@ -11539,14 +11548,352 @@
         <v>15</v>
       </c>
     </row>
+    <row r="1000" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1000">
+        <v>22</v>
+      </c>
+      <c r="B1000">
+        <v>10</v>
+      </c>
+      <c r="C1000" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1001">
+        <v>22</v>
+      </c>
+      <c r="B1001">
+        <v>10</v>
+      </c>
+      <c r="C1001" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1002">
+        <v>22</v>
+      </c>
+      <c r="B1002">
+        <v>11</v>
+      </c>
+      <c r="C1002" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1003">
+        <v>22</v>
+      </c>
+      <c r="B1003">
+        <v>11</v>
+      </c>
+      <c r="C1003" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1004">
+        <v>22</v>
+      </c>
+      <c r="B1004">
+        <v>11</v>
+      </c>
+      <c r="C1004" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1005">
+        <v>22</v>
+      </c>
+      <c r="B1005">
+        <v>11</v>
+      </c>
+      <c r="C1005" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1006">
+        <v>22</v>
+      </c>
+      <c r="B1006">
+        <v>11</v>
+      </c>
+      <c r="C1006" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1007">
+        <v>22</v>
+      </c>
+      <c r="B1007">
+        <v>11</v>
+      </c>
+      <c r="C1007" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1008">
+        <v>22</v>
+      </c>
+      <c r="B1008">
+        <v>11</v>
+      </c>
+      <c r="C1008" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1009">
+        <v>22</v>
+      </c>
+      <c r="B1009">
+        <v>11</v>
+      </c>
+      <c r="C1009" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1010">
+        <v>22</v>
+      </c>
+      <c r="B1010">
+        <v>11</v>
+      </c>
+      <c r="C1010" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1011">
+        <v>22</v>
+      </c>
+      <c r="B1011">
+        <v>11</v>
+      </c>
+      <c r="C1011" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1012">
+        <v>22</v>
+      </c>
+      <c r="B1012">
+        <v>11</v>
+      </c>
+      <c r="C1012" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1013">
+        <v>22</v>
+      </c>
+      <c r="B1013">
+        <v>11</v>
+      </c>
+      <c r="C1013" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1014">
+        <v>22</v>
+      </c>
+      <c r="B1014">
+        <v>11</v>
+      </c>
+      <c r="C1014" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1015">
+        <v>22</v>
+      </c>
+      <c r="B1015">
+        <v>11</v>
+      </c>
+      <c r="C1015" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1016">
+        <v>22</v>
+      </c>
+      <c r="B1016">
+        <v>11</v>
+      </c>
+      <c r="C1016" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1017">
+        <v>22</v>
+      </c>
+      <c r="B1017">
+        <v>11</v>
+      </c>
+      <c r="C1017" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1018">
+        <v>22</v>
+      </c>
+      <c r="B1018">
+        <v>11</v>
+      </c>
+      <c r="C1018" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1019">
+        <v>22</v>
+      </c>
+      <c r="B1019">
+        <v>11</v>
+      </c>
+      <c r="C1019" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1020">
+        <v>22</v>
+      </c>
+      <c r="B1020">
+        <v>11</v>
+      </c>
+      <c r="C1020" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1021">
+        <v>22</v>
+      </c>
+      <c r="B1021">
+        <v>11</v>
+      </c>
+      <c r="C1021" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1022">
+        <v>22</v>
+      </c>
+      <c r="B1022">
+        <v>11</v>
+      </c>
+      <c r="C1022" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1023">
+        <v>22</v>
+      </c>
+      <c r="B1023">
+        <v>11</v>
+      </c>
+      <c r="C1023" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1024">
+        <v>22</v>
+      </c>
+      <c r="B1024">
+        <v>11</v>
+      </c>
+      <c r="C1024" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1025">
+        <v>22</v>
+      </c>
+      <c r="B1025">
+        <v>11</v>
+      </c>
+      <c r="C1025" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1026">
+        <v>22</v>
+      </c>
+      <c r="B1026">
+        <v>11</v>
+      </c>
+      <c r="C1026" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1027">
+        <v>22</v>
+      </c>
+      <c r="B1027">
+        <v>11</v>
+      </c>
+      <c r="C1027" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1028">
+        <v>22</v>
+      </c>
+      <c r="B1028">
+        <v>11</v>
+      </c>
+      <c r="C1028" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1029">
+        <v>22</v>
+      </c>
+      <c r="B1029">
+        <v>11</v>
+      </c>
+      <c r="C1029" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1030">
+        <v>22</v>
+      </c>
+      <c r="B1030">
+        <v>11</v>
+      </c>
+      <c r="C1030" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C999" xr:uid="{22AB9C1C-DC34-4329-99EC-7D1CFEEBA821}">
-    <filterColumn colId="2">
+  <autoFilter ref="A1:C1001" xr:uid="{D56D1234-E9E6-4025-8B77-5AA3EA123576}">
+    <filterColumn colId="0">
       <filters>
-        <filter val="VIS300"/>
-        <filter val="VIS330"/>
-        <filter val="VIS340"/>
-        <filter val="VIS350"/>
+        <filter val="22"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Changed some basic data
</commit_message>
<xml_diff>
--- a/dataHistory.xlsx
+++ b/dataHistory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan_markvart\Documents\Python\Projects\InteractiveDashBoadr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3784C506-E292-464D-86A1-6D58B6A1DA2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80430E5-94C8-4848-9D88-EA5B379F66CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3028" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3086" uniqueCount="55">
   <si>
     <t>21</t>
   </si>
@@ -150,12 +150,51 @@
   <si>
     <t>VIS220</t>
   </si>
+  <si>
+    <t>VIS350</t>
+  </si>
+  <si>
+    <t>A 450</t>
+  </si>
+  <si>
+    <t>GS 300</t>
+  </si>
+  <si>
+    <t>A 550</t>
+  </si>
+  <si>
+    <t>GS 220</t>
+  </si>
+  <si>
+    <t>A 400</t>
+  </si>
+  <si>
+    <t>VIS 2000</t>
+  </si>
+  <si>
+    <t>DC 430</t>
+  </si>
+  <si>
+    <t>DC 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CM 220 </t>
+  </si>
+  <si>
+    <t>VIS 350</t>
+  </si>
+  <si>
+    <t>VIS 220</t>
+  </si>
+  <si>
+    <t>DC 410</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,12 +203,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -204,17 +256,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -551,10 +617,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C1030"/>
+  <dimension ref="A1:C1088"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A908" workbookViewId="0">
-      <selection activeCell="B1002" sqref="B1002:B1030"/>
+    <sheetView tabSelected="1" topLeftCell="A1063" workbookViewId="0">
+      <selection activeCell="F1082" sqref="F1082"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11887,6 +11953,644 @@
       </c>
       <c r="C1030" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1031">
+        <v>22</v>
+      </c>
+      <c r="B1031">
+        <v>12</v>
+      </c>
+      <c r="C1031" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1032">
+        <v>22</v>
+      </c>
+      <c r="B1032">
+        <v>12</v>
+      </c>
+      <c r="C1032" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1033">
+        <v>22</v>
+      </c>
+      <c r="B1033">
+        <v>12</v>
+      </c>
+      <c r="C1033" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1034">
+        <v>22</v>
+      </c>
+      <c r="B1034">
+        <v>12</v>
+      </c>
+      <c r="C1034" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1035">
+        <v>22</v>
+      </c>
+      <c r="B1035">
+        <v>12</v>
+      </c>
+      <c r="C1035" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1036">
+        <v>22</v>
+      </c>
+      <c r="B1036">
+        <v>12</v>
+      </c>
+      <c r="C1036" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1037">
+        <v>22</v>
+      </c>
+      <c r="B1037">
+        <v>12</v>
+      </c>
+      <c r="C1037" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1038">
+        <v>22</v>
+      </c>
+      <c r="B1038">
+        <v>12</v>
+      </c>
+      <c r="C1038" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1039">
+        <v>22</v>
+      </c>
+      <c r="B1039">
+        <v>12</v>
+      </c>
+      <c r="C1039" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1040">
+        <v>22</v>
+      </c>
+      <c r="B1040">
+        <v>12</v>
+      </c>
+      <c r="C1040" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1041">
+        <v>23</v>
+      </c>
+      <c r="B1041">
+        <v>1</v>
+      </c>
+      <c r="C1041" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1042">
+        <v>23</v>
+      </c>
+      <c r="B1042">
+        <v>1</v>
+      </c>
+      <c r="C1042" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1043">
+        <v>23</v>
+      </c>
+      <c r="B1043">
+        <v>1</v>
+      </c>
+      <c r="C1043" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1044">
+        <v>23</v>
+      </c>
+      <c r="B1044">
+        <v>1</v>
+      </c>
+      <c r="C1044" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1045">
+        <v>23</v>
+      </c>
+      <c r="B1045">
+        <v>1</v>
+      </c>
+      <c r="C1045" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1046">
+        <v>23</v>
+      </c>
+      <c r="B1046">
+        <v>1</v>
+      </c>
+      <c r="C1046" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1047">
+        <v>23</v>
+      </c>
+      <c r="B1047">
+        <v>1</v>
+      </c>
+      <c r="C1047" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1048">
+        <v>23</v>
+      </c>
+      <c r="B1048">
+        <v>1</v>
+      </c>
+      <c r="C1048" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1049">
+        <v>23</v>
+      </c>
+      <c r="B1049">
+        <v>1</v>
+      </c>
+      <c r="C1049" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1050">
+        <v>23</v>
+      </c>
+      <c r="B1050">
+        <v>1</v>
+      </c>
+      <c r="C1050" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1051">
+        <v>23</v>
+      </c>
+      <c r="B1051">
+        <v>1</v>
+      </c>
+      <c r="C1051" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1052">
+        <v>23</v>
+      </c>
+      <c r="B1052">
+        <v>1</v>
+      </c>
+      <c r="C1052" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1053">
+        <v>23</v>
+      </c>
+      <c r="B1053">
+        <v>1</v>
+      </c>
+      <c r="C1053" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1054">
+        <v>23</v>
+      </c>
+      <c r="B1054">
+        <v>1</v>
+      </c>
+      <c r="C1054" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1055">
+        <v>23</v>
+      </c>
+      <c r="B1055">
+        <v>1</v>
+      </c>
+      <c r="C1055" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1056">
+        <v>23</v>
+      </c>
+      <c r="B1056">
+        <v>1</v>
+      </c>
+      <c r="C1056" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1057">
+        <v>23</v>
+      </c>
+      <c r="B1057">
+        <v>1</v>
+      </c>
+      <c r="C1057" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1058">
+        <v>23</v>
+      </c>
+      <c r="B1058">
+        <v>1</v>
+      </c>
+      <c r="C1058" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1059">
+        <v>23</v>
+      </c>
+      <c r="B1059">
+        <v>1</v>
+      </c>
+      <c r="C1059" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1060">
+        <v>23</v>
+      </c>
+      <c r="B1060">
+        <v>1</v>
+      </c>
+      <c r="C1060" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1061">
+        <v>23</v>
+      </c>
+      <c r="B1061">
+        <v>1</v>
+      </c>
+      <c r="C1061" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1062">
+        <v>23</v>
+      </c>
+      <c r="B1062">
+        <v>1</v>
+      </c>
+      <c r="C1062" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1063">
+        <v>23</v>
+      </c>
+      <c r="B1063">
+        <v>1</v>
+      </c>
+      <c r="C1063" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1064">
+        <v>23</v>
+      </c>
+      <c r="B1064">
+        <v>1</v>
+      </c>
+      <c r="C1064" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1065">
+        <v>23</v>
+      </c>
+      <c r="B1065">
+        <v>1</v>
+      </c>
+      <c r="C1065" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1066">
+        <v>23</v>
+      </c>
+      <c r="B1066">
+        <v>1</v>
+      </c>
+      <c r="C1066" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1067">
+        <v>23</v>
+      </c>
+      <c r="B1067">
+        <v>1</v>
+      </c>
+      <c r="C1067" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1068">
+        <v>23</v>
+      </c>
+      <c r="B1068">
+        <v>1</v>
+      </c>
+      <c r="C1068" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1069">
+        <v>23</v>
+      </c>
+      <c r="B1069">
+        <v>1</v>
+      </c>
+      <c r="C1069" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1070">
+        <v>23</v>
+      </c>
+      <c r="B1070">
+        <v>1</v>
+      </c>
+      <c r="C1070" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1071">
+        <v>23</v>
+      </c>
+      <c r="B1071">
+        <v>1</v>
+      </c>
+      <c r="C1071" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1072">
+        <v>23</v>
+      </c>
+      <c r="B1072">
+        <v>1</v>
+      </c>
+      <c r="C1072" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1073">
+        <v>23</v>
+      </c>
+      <c r="B1073">
+        <v>2</v>
+      </c>
+      <c r="C1073" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1074">
+        <v>23</v>
+      </c>
+      <c r="B1074">
+        <v>2</v>
+      </c>
+      <c r="C1074" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1075">
+        <v>23</v>
+      </c>
+      <c r="B1075">
+        <v>2</v>
+      </c>
+      <c r="C1075" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1076">
+        <v>23</v>
+      </c>
+      <c r="B1076">
+        <v>2</v>
+      </c>
+      <c r="C1076" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1077">
+        <v>23</v>
+      </c>
+      <c r="B1077">
+        <v>2</v>
+      </c>
+      <c r="C1077" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1078">
+        <v>23</v>
+      </c>
+      <c r="B1078">
+        <v>2</v>
+      </c>
+      <c r="C1078" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1079">
+        <v>23</v>
+      </c>
+      <c r="B1079">
+        <v>2</v>
+      </c>
+      <c r="C1079" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1080">
+        <v>23</v>
+      </c>
+      <c r="B1080">
+        <v>2</v>
+      </c>
+      <c r="C1080" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1081">
+        <v>23</v>
+      </c>
+      <c r="B1081">
+        <v>2</v>
+      </c>
+      <c r="C1081" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1082">
+        <v>23</v>
+      </c>
+      <c r="B1082">
+        <v>2</v>
+      </c>
+      <c r="C1082" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1083">
+        <v>23</v>
+      </c>
+      <c r="B1083">
+        <v>2</v>
+      </c>
+      <c r="C1083" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1084">
+        <v>23</v>
+      </c>
+      <c r="B1084">
+        <v>2</v>
+      </c>
+      <c r="C1084" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1085">
+        <v>23</v>
+      </c>
+      <c r="B1085">
+        <v>2</v>
+      </c>
+      <c r="C1085" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1086">
+        <v>23</v>
+      </c>
+      <c r="B1086">
+        <v>2</v>
+      </c>
+      <c r="C1086" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1087">
+        <v>23</v>
+      </c>
+      <c r="B1087">
+        <v>2</v>
+      </c>
+      <c r="C1087" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1088">
+        <v>23</v>
+      </c>
+      <c r="B1088">
+        <v>2</v>
+      </c>
+      <c r="C1088" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -11898,5 +12602,6 @@
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added statistic by Month and Year
</commit_message>
<xml_diff>
--- a/dataHistory.xlsx
+++ b/dataHistory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan_markvart\Documents\Python\Projects\InteractiveDashBoadr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80430E5-94C8-4848-9D88-EA5B379F66CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750FAD0B-99D3-4FF2-9AEC-E285E755D3DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3086" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3177" uniqueCount="55">
   <si>
     <t>21</t>
   </si>
@@ -260,23 +260,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -619,8 +620,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:C1088"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1063" workbookViewId="0">
-      <selection activeCell="F1082" sqref="F1082"/>
+    <sheetView tabSelected="1" topLeftCell="A1062" workbookViewId="0">
+      <selection activeCell="B1073" sqref="B1073:B1088"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11615,30 +11616,30 @@
       </c>
     </row>
     <row r="1000" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1000">
-        <v>22</v>
-      </c>
-      <c r="B1000">
-        <v>10</v>
+      <c r="A1000" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1000" t="s">
+        <v>14</v>
       </c>
       <c r="C1000" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="1001" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1001">
-        <v>22</v>
-      </c>
-      <c r="B1001">
-        <v>10</v>
+      <c r="A1001" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1001" t="s">
+        <v>14</v>
       </c>
       <c r="C1001" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="1002" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1002">
-        <v>22</v>
+      <c r="A1002" t="s">
+        <v>2</v>
       </c>
       <c r="B1002">
         <v>11</v>
@@ -11648,8 +11649,8 @@
       </c>
     </row>
     <row r="1003" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1003">
-        <v>22</v>
+      <c r="A1003" t="s">
+        <v>2</v>
       </c>
       <c r="B1003">
         <v>11</v>
@@ -11659,8 +11660,8 @@
       </c>
     </row>
     <row r="1004" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1004">
-        <v>22</v>
+      <c r="A1004" t="s">
+        <v>2</v>
       </c>
       <c r="B1004">
         <v>11</v>
@@ -11670,8 +11671,8 @@
       </c>
     </row>
     <row r="1005" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1005">
-        <v>22</v>
+      <c r="A1005" t="s">
+        <v>2</v>
       </c>
       <c r="B1005">
         <v>11</v>
@@ -11681,8 +11682,8 @@
       </c>
     </row>
     <row r="1006" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1006">
-        <v>22</v>
+      <c r="A1006" t="s">
+        <v>2</v>
       </c>
       <c r="B1006">
         <v>11</v>
@@ -11692,8 +11693,8 @@
       </c>
     </row>
     <row r="1007" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1007">
-        <v>22</v>
+      <c r="A1007" t="s">
+        <v>2</v>
       </c>
       <c r="B1007">
         <v>11</v>
@@ -11703,8 +11704,8 @@
       </c>
     </row>
     <row r="1008" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1008">
-        <v>22</v>
+      <c r="A1008" t="s">
+        <v>2</v>
       </c>
       <c r="B1008">
         <v>11</v>
@@ -11714,8 +11715,8 @@
       </c>
     </row>
     <row r="1009" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1009">
-        <v>22</v>
+      <c r="A1009" t="s">
+        <v>2</v>
       </c>
       <c r="B1009">
         <v>11</v>
@@ -11725,8 +11726,8 @@
       </c>
     </row>
     <row r="1010" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1010">
-        <v>22</v>
+      <c r="A1010" t="s">
+        <v>2</v>
       </c>
       <c r="B1010">
         <v>11</v>
@@ -11736,8 +11737,8 @@
       </c>
     </row>
     <row r="1011" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1011">
-        <v>22</v>
+      <c r="A1011" t="s">
+        <v>2</v>
       </c>
       <c r="B1011">
         <v>11</v>
@@ -11747,8 +11748,8 @@
       </c>
     </row>
     <row r="1012" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1012">
-        <v>22</v>
+      <c r="A1012" t="s">
+        <v>2</v>
       </c>
       <c r="B1012">
         <v>11</v>
@@ -11758,8 +11759,8 @@
       </c>
     </row>
     <row r="1013" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1013">
-        <v>22</v>
+      <c r="A1013" t="s">
+        <v>2</v>
       </c>
       <c r="B1013">
         <v>11</v>
@@ -11769,8 +11770,8 @@
       </c>
     </row>
     <row r="1014" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1014">
-        <v>22</v>
+      <c r="A1014" t="s">
+        <v>2</v>
       </c>
       <c r="B1014">
         <v>11</v>
@@ -11780,8 +11781,8 @@
       </c>
     </row>
     <row r="1015" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1015">
-        <v>22</v>
+      <c r="A1015" t="s">
+        <v>2</v>
       </c>
       <c r="B1015">
         <v>11</v>
@@ -11791,8 +11792,8 @@
       </c>
     </row>
     <row r="1016" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1016">
-        <v>22</v>
+      <c r="A1016" t="s">
+        <v>2</v>
       </c>
       <c r="B1016">
         <v>11</v>
@@ -11802,8 +11803,8 @@
       </c>
     </row>
     <row r="1017" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1017">
-        <v>22</v>
+      <c r="A1017" t="s">
+        <v>2</v>
       </c>
       <c r="B1017">
         <v>11</v>
@@ -11813,8 +11814,8 @@
       </c>
     </row>
     <row r="1018" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1018">
-        <v>22</v>
+      <c r="A1018" t="s">
+        <v>2</v>
       </c>
       <c r="B1018">
         <v>11</v>
@@ -11824,8 +11825,8 @@
       </c>
     </row>
     <row r="1019" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1019">
-        <v>22</v>
+      <c r="A1019" t="s">
+        <v>2</v>
       </c>
       <c r="B1019">
         <v>11</v>
@@ -11835,8 +11836,8 @@
       </c>
     </row>
     <row r="1020" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1020">
-        <v>22</v>
+      <c r="A1020" t="s">
+        <v>2</v>
       </c>
       <c r="B1020">
         <v>11</v>
@@ -11846,8 +11847,8 @@
       </c>
     </row>
     <row r="1021" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1021">
-        <v>22</v>
+      <c r="A1021" t="s">
+        <v>2</v>
       </c>
       <c r="B1021">
         <v>11</v>
@@ -11857,8 +11858,8 @@
       </c>
     </row>
     <row r="1022" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1022">
-        <v>22</v>
+      <c r="A1022" t="s">
+        <v>2</v>
       </c>
       <c r="B1022">
         <v>11</v>
@@ -11868,8 +11869,8 @@
       </c>
     </row>
     <row r="1023" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1023">
-        <v>22</v>
+      <c r="A1023" t="s">
+        <v>2</v>
       </c>
       <c r="B1023">
         <v>11</v>
@@ -11879,8 +11880,8 @@
       </c>
     </row>
     <row r="1024" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1024">
-        <v>22</v>
+      <c r="A1024" t="s">
+        <v>2</v>
       </c>
       <c r="B1024">
         <v>11</v>
@@ -11890,8 +11891,8 @@
       </c>
     </row>
     <row r="1025" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1025">
-        <v>22</v>
+      <c r="A1025" t="s">
+        <v>2</v>
       </c>
       <c r="B1025">
         <v>11</v>
@@ -11901,8 +11902,8 @@
       </c>
     </row>
     <row r="1026" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1026">
-        <v>22</v>
+      <c r="A1026" t="s">
+        <v>2</v>
       </c>
       <c r="B1026">
         <v>11</v>
@@ -11912,8 +11913,8 @@
       </c>
     </row>
     <row r="1027" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1027">
-        <v>22</v>
+      <c r="A1027" t="s">
+        <v>2</v>
       </c>
       <c r="B1027">
         <v>11</v>
@@ -11923,8 +11924,8 @@
       </c>
     </row>
     <row r="1028" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1028">
-        <v>22</v>
+      <c r="A1028" t="s">
+        <v>2</v>
       </c>
       <c r="B1028">
         <v>11</v>
@@ -11934,8 +11935,8 @@
       </c>
     </row>
     <row r="1029" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1029">
-        <v>22</v>
+      <c r="A1029" t="s">
+        <v>2</v>
       </c>
       <c r="B1029">
         <v>11</v>
@@ -11945,8 +11946,8 @@
       </c>
     </row>
     <row r="1030" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1030">
-        <v>22</v>
+      <c r="A1030" t="s">
+        <v>2</v>
       </c>
       <c r="B1030">
         <v>11</v>
@@ -11956,8 +11957,8 @@
       </c>
     </row>
     <row r="1031" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1031">
-        <v>22</v>
+      <c r="A1031" t="s">
+        <v>2</v>
       </c>
       <c r="B1031">
         <v>12</v>
@@ -11967,8 +11968,8 @@
       </c>
     </row>
     <row r="1032" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1032">
-        <v>22</v>
+      <c r="A1032" t="s">
+        <v>2</v>
       </c>
       <c r="B1032">
         <v>12</v>
@@ -11978,8 +11979,8 @@
       </c>
     </row>
     <row r="1033" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1033">
-        <v>22</v>
+      <c r="A1033" t="s">
+        <v>2</v>
       </c>
       <c r="B1033">
         <v>12</v>
@@ -11989,8 +11990,8 @@
       </c>
     </row>
     <row r="1034" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1034">
-        <v>22</v>
+      <c r="A1034" t="s">
+        <v>2</v>
       </c>
       <c r="B1034">
         <v>12</v>
@@ -12000,8 +12001,8 @@
       </c>
     </row>
     <row r="1035" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1035">
-        <v>22</v>
+      <c r="A1035" t="s">
+        <v>2</v>
       </c>
       <c r="B1035">
         <v>12</v>
@@ -12011,8 +12012,8 @@
       </c>
     </row>
     <row r="1036" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1036">
-        <v>22</v>
+      <c r="A1036" t="s">
+        <v>2</v>
       </c>
       <c r="B1036">
         <v>12</v>
@@ -12022,8 +12023,8 @@
       </c>
     </row>
     <row r="1037" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1037">
-        <v>22</v>
+      <c r="A1037" t="s">
+        <v>2</v>
       </c>
       <c r="B1037">
         <v>12</v>
@@ -12033,8 +12034,8 @@
       </c>
     </row>
     <row r="1038" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1038">
-        <v>22</v>
+      <c r="A1038" t="s">
+        <v>2</v>
       </c>
       <c r="B1038">
         <v>12</v>
@@ -12044,8 +12045,8 @@
       </c>
     </row>
     <row r="1039" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1039">
-        <v>22</v>
+      <c r="A1039" t="s">
+        <v>2</v>
       </c>
       <c r="B1039">
         <v>12</v>
@@ -12055,8 +12056,8 @@
       </c>
     </row>
     <row r="1040" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1040">
-        <v>22</v>
+      <c r="A1040" t="s">
+        <v>2</v>
       </c>
       <c r="B1040">
         <v>12</v>
@@ -12069,8 +12070,8 @@
       <c r="A1041">
         <v>23</v>
       </c>
-      <c r="B1041">
-        <v>1</v>
+      <c r="B1041" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1041" s="2" t="s">
         <v>43</v>
@@ -12080,8 +12081,8 @@
       <c r="A1042">
         <v>23</v>
       </c>
-      <c r="B1042">
-        <v>1</v>
+      <c r="B1042" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1042" s="2" t="s">
         <v>44</v>
@@ -12091,8 +12092,8 @@
       <c r="A1043">
         <v>23</v>
       </c>
-      <c r="B1043">
-        <v>1</v>
+      <c r="B1043" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1043" s="2" t="s">
         <v>46</v>
@@ -12102,8 +12103,8 @@
       <c r="A1044">
         <v>23</v>
       </c>
-      <c r="B1044">
-        <v>1</v>
+      <c r="B1044" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1044" s="2" t="s">
         <v>47</v>
@@ -12113,8 +12114,8 @@
       <c r="A1045">
         <v>23</v>
       </c>
-      <c r="B1045">
-        <v>1</v>
+      <c r="B1045" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1045" s="2" t="s">
         <v>52</v>
@@ -12124,8 +12125,8 @@
       <c r="A1046">
         <v>23</v>
       </c>
-      <c r="B1046">
-        <v>1</v>
+      <c r="B1046" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1046" s="2" t="s">
         <v>48</v>
@@ -12135,8 +12136,8 @@
       <c r="A1047">
         <v>23</v>
       </c>
-      <c r="B1047">
-        <v>1</v>
+      <c r="B1047" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1047" s="2" t="s">
         <v>43</v>
@@ -12146,8 +12147,8 @@
       <c r="A1048">
         <v>23</v>
       </c>
-      <c r="B1048">
-        <v>1</v>
+      <c r="B1048" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1048" s="2" t="s">
         <v>46</v>
@@ -12157,8 +12158,8 @@
       <c r="A1049">
         <v>23</v>
       </c>
-      <c r="B1049">
-        <v>1</v>
+      <c r="B1049" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1049" s="2" t="s">
         <v>47</v>
@@ -12168,8 +12169,8 @@
       <c r="A1050">
         <v>23</v>
       </c>
-      <c r="B1050">
-        <v>1</v>
+      <c r="B1050" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1050" s="2" t="s">
         <v>47</v>
@@ -12179,8 +12180,8 @@
       <c r="A1051">
         <v>23</v>
       </c>
-      <c r="B1051">
-        <v>1</v>
+      <c r="B1051" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1051" s="2" t="s">
         <v>49</v>
@@ -12190,8 +12191,8 @@
       <c r="A1052">
         <v>23</v>
       </c>
-      <c r="B1052">
-        <v>1</v>
+      <c r="B1052" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1052" s="2" t="s">
         <v>43</v>
@@ -12201,8 +12202,8 @@
       <c r="A1053">
         <v>23</v>
       </c>
-      <c r="B1053">
-        <v>1</v>
+      <c r="B1053" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1053" s="2" t="s">
         <v>47</v>
@@ -12212,8 +12213,8 @@
       <c r="A1054">
         <v>23</v>
       </c>
-      <c r="B1054">
-        <v>1</v>
+      <c r="B1054" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1054" s="2" t="s">
         <v>46</v>
@@ -12223,8 +12224,8 @@
       <c r="A1055">
         <v>23</v>
       </c>
-      <c r="B1055">
-        <v>1</v>
+      <c r="B1055" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1055" s="2" t="s">
         <v>44</v>
@@ -12234,8 +12235,8 @@
       <c r="A1056">
         <v>23</v>
       </c>
-      <c r="B1056">
-        <v>1</v>
+      <c r="B1056" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1056" s="2" t="s">
         <v>44</v>
@@ -12245,8 +12246,8 @@
       <c r="A1057">
         <v>23</v>
       </c>
-      <c r="B1057">
-        <v>1</v>
+      <c r="B1057" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1057" s="2" t="s">
         <v>43</v>
@@ -12256,8 +12257,8 @@
       <c r="A1058">
         <v>23</v>
       </c>
-      <c r="B1058">
-        <v>1</v>
+      <c r="B1058" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1058" s="3" t="s">
         <v>46</v>
@@ -12267,8 +12268,8 @@
       <c r="A1059">
         <v>23</v>
       </c>
-      <c r="B1059">
-        <v>1</v>
+      <c r="B1059" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1059" s="3" t="s">
         <v>45</v>
@@ -12278,8 +12279,8 @@
       <c r="A1060">
         <v>23</v>
       </c>
-      <c r="B1060">
-        <v>1</v>
+      <c r="B1060" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1060" s="2" t="s">
         <v>44</v>
@@ -12289,8 +12290,8 @@
       <c r="A1061">
         <v>23</v>
       </c>
-      <c r="B1061">
-        <v>1</v>
+      <c r="B1061" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1061" s="2" t="s">
         <v>47</v>
@@ -12300,8 +12301,8 @@
       <c r="A1062">
         <v>23</v>
       </c>
-      <c r="B1062">
-        <v>1</v>
+      <c r="B1062" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1062" s="3" t="s">
         <v>46</v>
@@ -12311,8 +12312,8 @@
       <c r="A1063">
         <v>23</v>
       </c>
-      <c r="B1063">
-        <v>1</v>
+      <c r="B1063" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1063" s="3" t="s">
         <v>43</v>
@@ -12322,8 +12323,8 @@
       <c r="A1064">
         <v>23</v>
       </c>
-      <c r="B1064">
-        <v>1</v>
+      <c r="B1064" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1064" s="3" t="s">
         <v>45</v>
@@ -12333,8 +12334,8 @@
       <c r="A1065">
         <v>23</v>
       </c>
-      <c r="B1065">
-        <v>1</v>
+      <c r="B1065" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1065" s="3" t="s">
         <v>50</v>
@@ -12344,8 +12345,8 @@
       <c r="A1066">
         <v>23</v>
       </c>
-      <c r="B1066">
-        <v>1</v>
+      <c r="B1066" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1066" s="2" t="s">
         <v>51</v>
@@ -12355,8 +12356,8 @@
       <c r="A1067">
         <v>23</v>
       </c>
-      <c r="B1067">
-        <v>1</v>
+      <c r="B1067" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1067" s="3" t="s">
         <v>47</v>
@@ -12366,8 +12367,8 @@
       <c r="A1068">
         <v>23</v>
       </c>
-      <c r="B1068">
-        <v>1</v>
+      <c r="B1068" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1068" s="4" t="s">
         <v>50</v>
@@ -12377,8 +12378,8 @@
       <c r="A1069">
         <v>23</v>
       </c>
-      <c r="B1069">
-        <v>1</v>
+      <c r="B1069" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1069" s="5" t="s">
         <v>48</v>
@@ -12388,8 +12389,8 @@
       <c r="A1070">
         <v>23</v>
       </c>
-      <c r="B1070">
-        <v>1</v>
+      <c r="B1070" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1070" s="2" t="s">
         <v>46</v>
@@ -12399,8 +12400,8 @@
       <c r="A1071">
         <v>23</v>
       </c>
-      <c r="B1071">
-        <v>1</v>
+      <c r="B1071" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1071" s="2" t="s">
         <v>46</v>
@@ -12410,8 +12411,8 @@
       <c r="A1072">
         <v>23</v>
       </c>
-      <c r="B1072">
-        <v>1</v>
+      <c r="B1072" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C1072" s="2" t="s">
         <v>44</v>
@@ -12421,8 +12422,8 @@
       <c r="A1073">
         <v>23</v>
       </c>
-      <c r="B1073">
-        <v>2</v>
+      <c r="B1073" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="C1073" s="2" t="s">
         <v>43</v>
@@ -12432,8 +12433,8 @@
       <c r="A1074">
         <v>23</v>
       </c>
-      <c r="B1074">
-        <v>2</v>
+      <c r="B1074" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="C1074" s="2" t="s">
         <v>47</v>
@@ -12443,8 +12444,8 @@
       <c r="A1075">
         <v>23</v>
       </c>
-      <c r="B1075">
-        <v>2</v>
+      <c r="B1075" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="C1075" s="2" t="s">
         <v>46</v>
@@ -12454,8 +12455,8 @@
       <c r="A1076">
         <v>23</v>
       </c>
-      <c r="B1076">
-        <v>2</v>
+      <c r="B1076" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="C1076" s="2" t="s">
         <v>44</v>
@@ -12465,8 +12466,8 @@
       <c r="A1077">
         <v>23</v>
       </c>
-      <c r="B1077">
-        <v>2</v>
+      <c r="B1077" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="C1077" s="2" t="s">
         <v>44</v>
@@ -12476,8 +12477,8 @@
       <c r="A1078">
         <v>23</v>
       </c>
-      <c r="B1078">
-        <v>2</v>
+      <c r="B1078" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="C1078" s="2" t="s">
         <v>47</v>
@@ -12487,8 +12488,8 @@
       <c r="A1079">
         <v>23</v>
       </c>
-      <c r="B1079">
-        <v>2</v>
+      <c r="B1079" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="C1079" s="2" t="s">
         <v>43</v>
@@ -12498,8 +12499,8 @@
       <c r="A1080">
         <v>23</v>
       </c>
-      <c r="B1080">
-        <v>2</v>
+      <c r="B1080" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="C1080" s="2" t="s">
         <v>54</v>
@@ -12509,8 +12510,8 @@
       <c r="A1081">
         <v>23</v>
       </c>
-      <c r="B1081">
-        <v>2</v>
+      <c r="B1081" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="C1081" s="2" t="s">
         <v>47</v>
@@ -12520,8 +12521,8 @@
       <c r="A1082">
         <v>23</v>
       </c>
-      <c r="B1082">
-        <v>2</v>
+      <c r="B1082" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="C1082" s="2" t="s">
         <v>53</v>
@@ -12531,8 +12532,8 @@
       <c r="A1083">
         <v>23</v>
       </c>
-      <c r="B1083">
-        <v>2</v>
+      <c r="B1083" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="C1083" s="2" t="s">
         <v>47</v>
@@ -12542,8 +12543,8 @@
       <c r="A1084">
         <v>23</v>
       </c>
-      <c r="B1084">
-        <v>2</v>
+      <c r="B1084" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="C1084" s="2" t="s">
         <v>48</v>
@@ -12553,8 +12554,8 @@
       <c r="A1085">
         <v>23</v>
       </c>
-      <c r="B1085">
-        <v>2</v>
+      <c r="B1085" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="C1085" s="2" t="s">
         <v>52</v>
@@ -12564,8 +12565,8 @@
       <c r="A1086">
         <v>23</v>
       </c>
-      <c r="B1086">
-        <v>2</v>
+      <c r="B1086" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="C1086" s="2" t="s">
         <v>46</v>
@@ -12575,8 +12576,8 @@
       <c r="A1087">
         <v>23</v>
       </c>
-      <c r="B1087">
-        <v>2</v>
+      <c r="B1087" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="C1087" s="2" t="s">
         <v>46</v>
@@ -12586,8 +12587,8 @@
       <c r="A1088">
         <v>23</v>
       </c>
-      <c r="B1088">
-        <v>2</v>
+      <c r="B1088" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="C1088" s="2" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
Feat: Connect page "Statistiak celkova" to MongoDB
</commit_message>
<xml_diff>
--- a/dataHistory.xlsx
+++ b/dataHistory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan_markvart\Documents\Python\Projects\InteractiveDashBoadr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBD1CCB-1EEA-47CA-BBA2-73F9AA121425}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6405004-C70F-4F4D-9C6D-22F78B644C73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3223" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3973" uniqueCount="42">
   <si>
     <t>21</t>
   </si>
@@ -144,18 +144,31 @@
   <si>
     <t>23</t>
   </si>
+  <si>
+    <t>GS 220</t>
+  </si>
+  <si>
+    <t>DC420</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
@@ -213,26 +226,29 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -572,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1089"/>
+  <dimension ref="A1:E1338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1077" workbookViewId="0">
-      <selection activeCell="C1089" sqref="C1089"/>
+    <sheetView tabSelected="1" topLeftCell="A1294" workbookViewId="0">
+      <selection activeCell="F1331" sqref="F1331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12548,9 +12564,2796 @@
         <v>31</v>
       </c>
     </row>
-    <row r="1089" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B1089" s="6"/>
-      <c r="C1089" s="2"/>
+    <row r="1089" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1089" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1089" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1089" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1090" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1090" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1090" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1091" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1091" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1091" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1092" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1092" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1092" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1093" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1093" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1093" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1094" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1094" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1094" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1095" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1095" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1095" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1096" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1096" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1096" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1097" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1097" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1097" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1098" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1098" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1098" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1099" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1099" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1099" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1100" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1100" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1100" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1101" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1101" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1101" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1102" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1102" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1102" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1103" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1103" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1103" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1104" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1104" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1104" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1105" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1105" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1105" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1106" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1106" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1106" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1107" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1107" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1107" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1108" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1108" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1108" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1109" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1109" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1109" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1110" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1110" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1110" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1111" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1111" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1111" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1112" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1112" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1112" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1113" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1113" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1113" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1114" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1114" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1114" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1115" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1115" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1115" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1116" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1116" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1116" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1117" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1117" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1117" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1118" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1118" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1118" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1119" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1119" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1119" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1120" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1120" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1120" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1121" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1121" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1121" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1122" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1122" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1122" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1123" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1123" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1123" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1124" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1124" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1124" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1125" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1125" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1125" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1126" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1126" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1126" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1127" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1127" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1127" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1128" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1128" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1128" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1129" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1129" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1129" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1130" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1130" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1130" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1131" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1131" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1131" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1132" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1132" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1132" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1133" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1133" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1133" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1134" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1134" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1134" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1135" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1135" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1135" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1136" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1136" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1136" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1137" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1137" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1137" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1138" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1138" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1138" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1139" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1139" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1139" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1140" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1140" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1140" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1141" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1141" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1141" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1142" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1142" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1142" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1143" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1143" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1143" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1144" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1144" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1144" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1145" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1145" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1145" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1146" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1146" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1146" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1147" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1147" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1147" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1148" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1148" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1148" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1149" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1149" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1149" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1150" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1150" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1150" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1151" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1151" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1151" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1152" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1152" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1152" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1153" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1153" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1153" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1154" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1154" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1154" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1155" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1155" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1155" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1156" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1156" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1156" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1157" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1157" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1157" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1158" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1158" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1158" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1159" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1159" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1159" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1160" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1160" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1160" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1161" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1161" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1161" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1162" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1162" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1162" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1163" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1163" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1163" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1164" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1164" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1164" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1165" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1165" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1165" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1166" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1166" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1166" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1167" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1167" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1167" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1168" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1168" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1168" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1169" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1169" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1169" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1170" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1170" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1170" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1171" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1171" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1171" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1172" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1172" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1172" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1173" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1173" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1173" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1174" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1174" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1174" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1175" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1175" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1175" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1176" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1176" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1176" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1177" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1177" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1177" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1178" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1178" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1178" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1179" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1179" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1179" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1180" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1180" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1180" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1181" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1181" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1181" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1182" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1182" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1182" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1183" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1183" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1183" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1184" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1184" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1184" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1185" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1185" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1185" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1186" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1186" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1186" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1187" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1187" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1187" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1188" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1188" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1188" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1189" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1189" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1189" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1190" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1190" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1190" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1191" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1191" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1191" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1192" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1192" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1192" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1193" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1193" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1193" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1193" s="2"/>
+    </row>
+    <row r="1194" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1194" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1194" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1194" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1194" s="2"/>
+    </row>
+    <row r="1195" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1195" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1195" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1195" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1195" s="2"/>
+    </row>
+    <row r="1196" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1196" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1196" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1196" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1196" s="2"/>
+    </row>
+    <row r="1197" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1197" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1197" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1197" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1197" s="5"/>
+    </row>
+    <row r="1198" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1198" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1198" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1198" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1198" s="2"/>
+    </row>
+    <row r="1199" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1199" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1199" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1199" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1199" s="2"/>
+    </row>
+    <row r="1200" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1200" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1200" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1200" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1200" s="2"/>
+    </row>
+    <row r="1201" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1201" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1201" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1201" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1201" s="2"/>
+    </row>
+    <row r="1202" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1202" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1202" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1202" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1202" s="2"/>
+    </row>
+    <row r="1203" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1203" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1203" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1203" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1204" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1204" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1204" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1205" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1205" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1205" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1206" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1206" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1206" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1207" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1207" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1207" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1208" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1208" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1208" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1209" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1209" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1209" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1210" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1210" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1210" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1211" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1211" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1211" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1212" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1212" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1212" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1213" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1213" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1213" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1213" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1214" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1214" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1214" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1215" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1215" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1215" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1215" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1216" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1216" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1216" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1216" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1217" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1217" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1217" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1218" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1218" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1218" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1219" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1219" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1219" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1220" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1220" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1220" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1221" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1221" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1221" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1222" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1222" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1222" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1223" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1223" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1223" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1224" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1224" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1224" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1225" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1225" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1225" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1226" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1226" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1226" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1227" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1227" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1227" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1227" s="2"/>
+    </row>
+    <row r="1228" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1228" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1228" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1228" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1228" s="2"/>
+    </row>
+    <row r="1229" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1229" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1229" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1229" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1229" s="2"/>
+    </row>
+    <row r="1230" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1230" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1230" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1230" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1230" s="2"/>
+    </row>
+    <row r="1231" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1231" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1231" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1231" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1231" s="5"/>
+    </row>
+    <row r="1232" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1232" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1232" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1232" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1232" s="2"/>
+    </row>
+    <row r="1233" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1233" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1233" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1233" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1233" s="2"/>
+    </row>
+    <row r="1234" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1234" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1234" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1234" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1234" s="2"/>
+    </row>
+    <row r="1235" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1235" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1235" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1235" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1235" s="2"/>
+    </row>
+    <row r="1236" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1236" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1236" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1236" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1236" s="2"/>
+    </row>
+    <row r="1237" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1237" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1237" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1237" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1238" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1238" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1238" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1239" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1239" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1239" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1240" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1240" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1240" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1241" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1241" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1241" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1242" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1242" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1242" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1243" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1243" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1243" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1244" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1244" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1244" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1245" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1245" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1245" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1246" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1246" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1246" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1247" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1247" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1247" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1248" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1248" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1248" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1249" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1249" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1249" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1250" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1250" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1250" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1250" s="2"/>
+    </row>
+    <row r="1251" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1251" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1251" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1251" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1251" s="2"/>
+    </row>
+    <row r="1252" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1252" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1252" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1252" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1252" s="2"/>
+    </row>
+    <row r="1253" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1253" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1253" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1253" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1253" s="2"/>
+    </row>
+    <row r="1254" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1254" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1254" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1254" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1254" s="5"/>
+    </row>
+    <row r="1255" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1255" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1255" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1255" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1255" s="2"/>
+    </row>
+    <row r="1256" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1256" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1256" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1256" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1256" s="2"/>
+    </row>
+    <row r="1257" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1257" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1257" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1257" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1257" s="2"/>
+    </row>
+    <row r="1258" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1258" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1258" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1258" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1258" s="2"/>
+    </row>
+    <row r="1259" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1259" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1259" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1259" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1259" s="2"/>
+    </row>
+    <row r="1260" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1260" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1260" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1260" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1260" s="2"/>
+    </row>
+    <row r="1261" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1261" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1261" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1261" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1262" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1262" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1262" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1263" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1263" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1263" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1264" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1264" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1264" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1265" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1265" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1265" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1266" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1266" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1266" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1267" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1267" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1267" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1268" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1268" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1268" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1269" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1269" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1269" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1270" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1270" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1270" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1271" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1271" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1271" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1272" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1272" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1272" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1273" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1273" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1273" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1274" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1274" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1274" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1275" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1275" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1275" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1276" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1276" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1276" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1277" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1277" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1277" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1278" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1278" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1278" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1279" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1279" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1279" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1280" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1280" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1280" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1281" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1281" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1281" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1282" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1282" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1282" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1283" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1283" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1283" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1284" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1284" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1284" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1285" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1285" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1285" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1286" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1286" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1286" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1286" s="2"/>
+    </row>
+    <row r="1287" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1287" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1287" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1287" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1287" s="2"/>
+    </row>
+    <row r="1288" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1288" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1288" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1288" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1288" s="2"/>
+    </row>
+    <row r="1289" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1289" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1289" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1289" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1289" s="5"/>
+    </row>
+    <row r="1290" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1290" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1290" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1290" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1290" s="2"/>
+    </row>
+    <row r="1291" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1291" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1291" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1291" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1291" s="2"/>
+    </row>
+    <row r="1292" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1292" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1292" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1292" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1292" s="2"/>
+    </row>
+    <row r="1293" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1293" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1293" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1293" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1293" s="2"/>
+    </row>
+    <row r="1294" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1294" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1294" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1294" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1294" s="2"/>
+    </row>
+    <row r="1295" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1295" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1295" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1295" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1295" s="2"/>
+    </row>
+    <row r="1296" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1296" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1296" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1296" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1297" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1297" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1297" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1298" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1298" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1298" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1299" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1299" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1299" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1300" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1300" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1300" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1301" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1301" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1301" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1302" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1302" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1302" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1303" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1303" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1303" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1304" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1304" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1304" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1304" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1305" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1305" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1305" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1306" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1306" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1306" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1307" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1307" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1307" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1308" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1308" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1308" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1309" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1309" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1309" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1310" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1310" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1310" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1311" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1311" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1311" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1312" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1312" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1312" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1313" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1313" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1313" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1314" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1314" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1314" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1315" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1315" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1315" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1316" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1316" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1316" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1317" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1317" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1317" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1318" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1318" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1318" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1319" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1319" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1319" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1320" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1320" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1320" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1321" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1321" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1321" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1322" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1322" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1322" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1323" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1323" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1323" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1324" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1324" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1324" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1325" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1325" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1325" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1326" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1326" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1326" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1327" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1327" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1327" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1328" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1328" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1328" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1329" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1329" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1329" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1330" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1330" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1330" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1331" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1331" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1331" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1332" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1332" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1332" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1333" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1333" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1333" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1334" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1334" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1334" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1335" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1335" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1335" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1336" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1336" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1336" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1337" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1337" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1337" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1338" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1338" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1338" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1082" xr:uid="{D56D1234-E9E6-4025-8B77-5AA3EA123576}"/>

</xml_diff>